<commit_message>
Actualización de la planilla de turnos
</commit_message>
<xml_diff>
--- a/lista_de_turnos.xlsx
+++ b/lista_de_turnos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos_I\Documents\proyectos de python\turnos_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74748DD0-EF64-4578-AE56-4015BAA2AE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{801DD413-14BC-4705-85AA-9D3591B59799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{EDD43B73-A7BB-452E-AC1E-9132C672CC1E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="55">
   <si>
     <t>inicio</t>
   </si>
@@ -131,9 +131,6 @@
     <t>18.392.207 -6</t>
   </si>
   <si>
-    <t xml:space="preserve"> 16.366.615-4</t>
-  </si>
-  <si>
     <t>19.812.071-5</t>
   </si>
   <si>
@@ -149,9 +146,6 @@
     <t>18.953.130-3</t>
   </si>
   <si>
-    <t xml:space="preserve"> 15.343.687-8</t>
-  </si>
-  <si>
     <t>16.751.516 -9</t>
   </si>
   <si>
@@ -188,13 +182,25 @@
     <t>20.014.370-1</t>
   </si>
   <si>
-    <t xml:space="preserve">16.790.074-7 </t>
-  </si>
-  <si>
     <t>17.045.023-K</t>
   </si>
   <si>
     <t>rut</t>
+  </si>
+  <si>
+    <t>16.759.697-5</t>
+  </si>
+  <si>
+    <t>16.751.516-9</t>
+  </si>
+  <si>
+    <t>16.366.615-4</t>
+  </si>
+  <si>
+    <t>15.343.687-8</t>
+  </si>
+  <si>
+    <t>16.790.074-7</t>
   </si>
 </sst>
 </file>
@@ -722,7 +728,7 @@
   <dimension ref="A1:E78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -737,7 +743,7 @@
         <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>22</v>
@@ -788,7 +794,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -805,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -822,7 +828,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -839,7 +845,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -856,7 +862,7 @@
         <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -873,7 +879,7 @@
         <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -890,7 +896,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -907,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>38</v>
+        <v>51</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -924,7 +930,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -941,7 +947,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -958,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -975,7 +981,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -992,7 +998,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1009,7 +1015,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>18</v>
@@ -1026,7 +1032,7 @@
         <v>25</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>18</v>
@@ -1043,7 +1049,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>18</v>
@@ -1060,7 +1066,7 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>18</v>
@@ -1077,7 +1083,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>18</v>
@@ -1094,7 +1100,7 @@
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>18</v>
@@ -1111,7 +1117,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>18</v>
@@ -1128,7 +1134,7 @@
         <v>26</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>18</v>
@@ -1145,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>18</v>
@@ -1162,7 +1168,7 @@
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>18</v>
@@ -1179,7 +1185,7 @@
         <v>6</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>18</v>
@@ -1196,7 +1202,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
@@ -1213,7 +1219,7 @@
         <v>17</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>19</v>
@@ -1247,7 +1253,7 @@
         <v>20</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>19</v>
@@ -1264,7 +1270,7 @@
         <v>7</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>19</v>
@@ -1281,7 +1287,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -1298,7 +1304,7 @@
         <v>25</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -1315,7 +1321,7 @@
         <v>14</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="1">
         <v>2</v>
@@ -1332,7 +1338,7 @@
         <v>27</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
@@ -1349,7 +1355,7 @@
         <v>2</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
@@ -1366,7 +1372,7 @@
         <v>5</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -1400,7 +1406,7 @@
         <v>10</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -1417,7 +1423,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
@@ -1434,7 +1440,7 @@
         <v>11</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1451,7 +1457,7 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C43" s="1">
         <v>2</v>
@@ -1468,7 +1474,7 @@
         <v>26</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
@@ -1485,7 +1491,7 @@
         <v>20</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
@@ -1502,7 +1508,7 @@
         <v>21</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
@@ -1519,7 +1525,7 @@
         <v>9</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C47" s="1">
         <v>2</v>
@@ -1570,7 +1576,7 @@
         <v>8</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>31</v>
+        <v>52</v>
       </c>
       <c r="C50" s="1">
         <v>3</v>
@@ -1587,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C51" s="1">
         <v>3</v>
@@ -1604,7 +1610,7 @@
         <v>14</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C52" s="1">
         <v>3</v>
@@ -1621,7 +1627,7 @@
         <v>27</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C53" s="1">
         <v>3</v>
@@ -1638,7 +1644,7 @@
         <v>2</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C54" s="1">
         <v>3</v>
@@ -1655,7 +1661,7 @@
         <v>16</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C55" s="1">
         <v>3</v>
@@ -1672,7 +1678,7 @@
         <v>10</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C56" s="1">
         <v>3</v>
@@ -1689,7 +1695,7 @@
         <v>13</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C57" s="1">
         <v>3</v>
@@ -1706,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C58" s="1">
         <v>3</v>
@@ -1723,7 +1729,7 @@
         <v>26</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C59" s="1">
         <v>3</v>
@@ -1740,7 +1746,7 @@
         <v>20</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C60" s="1">
         <v>3</v>
@@ -1757,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C61" s="1">
         <v>3</v>
@@ -1774,7 +1780,7 @@
         <v>6</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C62" s="1">
         <v>3</v>
@@ -1825,7 +1831,7 @@
         <v>4</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C65" s="1">
         <v>4</v>
@@ -1842,7 +1848,7 @@
         <v>25</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C66" s="1">
         <v>4</v>
@@ -1859,7 +1865,7 @@
         <v>14</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C67" s="1">
         <v>4</v>
@@ -1876,7 +1882,7 @@
         <v>2</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C68" s="1">
         <v>4</v>
@@ -1893,7 +1899,7 @@
         <v>28</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C69" s="1">
         <v>4</v>
@@ -1910,7 +1916,7 @@
         <v>5</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C70" s="1">
         <v>4</v>
@@ -1927,7 +1933,7 @@
         <v>13</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1">
         <v>4</v>
@@ -1944,7 +1950,7 @@
         <v>3</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C72" s="1">
         <v>4</v>
@@ -1961,7 +1967,7 @@
         <v>11</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="C73" s="1">
         <v>4</v>
@@ -1978,7 +1984,7 @@
         <v>1</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C74" s="1">
         <v>4</v>
@@ -1995,7 +2001,7 @@
         <v>26</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C75" s="1">
         <v>4</v>
@@ -2012,7 +2018,7 @@
         <v>20</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C76" s="1">
         <v>4</v>
@@ -2029,7 +2035,7 @@
         <v>21</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C77" s="1">
         <v>4</v>
@@ -2046,7 +2052,7 @@
         <v>6</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C78" s="1">
         <v>4</v>
@@ -2068,6 +2074,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3a1d6b35-d74b-4e6e-9e33-1d286005928a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d6b7251-971b-421d-9ba0-6b2023d693f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AB947A98EBEFFA45B551653668971F36" ma:contentTypeVersion="23" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4a71894c677265028c25fea40c469a7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a1d6b35-d74b-4e6e-9e33-1d286005928a" xmlns:ns3="0d6b7251-971b-421d-9ba0-6b2023d693f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3237d064db606537c4e696f73d4d905c" ns2:_="" ns3:_="">
     <xsd:import namespace="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
@@ -2322,41 +2348,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3a1d6b35-d74b-4e6e-9e33-1d286005928a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d6b7251-971b-421d-9ba0-6b2023d693f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B7F710-491D-49B9-894A-18729FC96536}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A1A307-8C34-4E84-BA59-2F0A23A06A42}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
-    <ds:schemaRef ds:uri="0d6b7251-971b-421d-9ba0-6b2023d693f9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2379,9 +2374,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A1A307-8C34-4E84-BA59-2F0A23A06A42}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B7F710-491D-49B9-894A-18729FC96536}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
+    <ds:schemaRef ds:uri="0d6b7251-971b-421d-9ba0-6b2023d693f9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Actualización de turnos en lista_de_turnos.xlsx
</commit_message>
<xml_diff>
--- a/lista_de_turnos.xlsx
+++ b/lista_de_turnos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos_I\Documents\proyectos de python\turnos_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE19433-B966-479E-88B2-DB980D371F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AA1A4B-B44B-480B-9424-4E17BAF0170E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="16440" xr2:uid="{EDD43B73-A7BB-452E-AC1E-9132C672CC1E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{EDD43B73-A7BB-452E-AC1E-9132C672CC1E}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="7" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="55">
   <si>
     <t>inicio</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Cristian Sepúlveda</t>
   </si>
   <si>
-    <t>Albert Neira</t>
-  </si>
-  <si>
     <t>Valentina Neupert</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>17.408.267-7</t>
   </si>
   <si>
-    <t>16.466.873-8</t>
-  </si>
-  <si>
     <t>14.074.041-1</t>
   </si>
   <si>
@@ -195,6 +189,18 @@
   </si>
   <si>
     <t>18.392.207-6</t>
+  </si>
+  <si>
+    <t>16.755.783-k</t>
+  </si>
+  <si>
+    <t>Jairo Delgado</t>
+  </si>
+  <si>
+    <t>Alondra José Landeros</t>
+  </si>
+  <si>
+    <t>Estudio chinchillas mayo</t>
   </si>
 </sst>
 </file>
@@ -244,7 +250,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -253,6 +259,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,8 +400,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D95D8EF4-2740-4C76-9EF0-613AE15FA685}" name="Tabla1" displayName="Tabla1" ref="A1:E77" totalsRowShown="0">
-  <autoFilter ref="A1:E77" xr:uid="{D95D8EF4-2740-4C76-9EF0-613AE15FA685}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D95D8EF4-2740-4C76-9EF0-613AE15FA685}" name="Tabla1" displayName="Tabla1" ref="A1:E84" totalsRowShown="0">
+  <autoFilter ref="A1:E84" xr:uid="{D95D8EF4-2740-4C76-9EF0-613AE15FA685}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{B36830FA-78BB-4264-97CD-47B06E368413}" name="Nombre" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C145A84A-77B6-40E3-8776-445244187024}" name="rut" dataDxfId="3"/>
@@ -719,42 +731,42 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBBD1A30-C2F7-4FA2-886C-6AF90F726A62}">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A84" sqref="A84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="18" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -768,10 +780,10 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
@@ -785,10 +797,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -802,10 +814,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" s="1">
         <v>1</v>
@@ -819,10 +831,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
@@ -839,7 +851,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="1">
         <v>1</v>
@@ -853,10 +865,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
@@ -870,10 +882,10 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C9" s="1">
         <v>1</v>
@@ -887,10 +899,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
@@ -907,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C11" s="1">
         <v>1</v>
@@ -921,10 +933,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
@@ -938,10 +950,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1">
         <v>1</v>
@@ -958,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
@@ -975,7 +987,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15" s="1">
         <v>1</v>
@@ -992,7 +1004,7 @@
         <v>3</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C16" s="1">
         <v>1</v>
@@ -1009,10 +1021,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="3">
         <v>45768</v>
@@ -1023,13 +1035,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D18" s="3">
         <v>45768</v>
@@ -1040,13 +1052,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D19" s="3">
         <v>45768</v>
@@ -1060,10 +1072,10 @@
         <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D20" s="3">
         <v>45768</v>
@@ -1074,13 +1086,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D21" s="3">
         <v>45768</v>
@@ -1091,13 +1103,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D22" s="3">
         <v>45768</v>
@@ -1111,10 +1123,10 @@
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D23" s="3">
         <v>45768</v>
@@ -1125,13 +1137,13 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D24" s="3">
         <v>45768</v>
@@ -1142,13 +1154,13 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D25" s="3">
         <v>45768</v>
@@ -1159,13 +1171,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D26" s="3">
         <v>45768</v>
@@ -1176,13 +1188,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D27" s="3">
         <v>45768</v>
@@ -1193,30 +1205,30 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="3">
-        <v>45768</v>
+        <v>45774</v>
       </c>
       <c r="E28" s="3">
-        <v>45774</v>
+        <v>45780</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D29" s="3">
         <v>45774</v>
@@ -1227,13 +1239,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D30" s="3">
         <v>45774</v>
@@ -1243,14 +1255,14 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
-        <v>20</v>
+      <c r="A31" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D31" s="3">
         <v>45774</v>
@@ -1264,7 +1276,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C32" s="1">
         <v>2</v>
@@ -1278,10 +1290,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C33" s="1">
         <v>2</v>
@@ -1295,10 +1307,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C34" s="1">
         <v>2</v>
@@ -1312,10 +1324,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C35" s="1">
         <v>2</v>
@@ -1332,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C36" s="1">
         <v>2</v>
@@ -1349,7 +1361,7 @@
         <v>5</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1">
         <v>2</v>
@@ -1363,10 +1375,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C38" s="1">
         <v>2</v>
@@ -1380,10 +1392,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C39" s="1">
         <v>2</v>
@@ -1397,10 +1409,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="1">
         <v>2</v>
@@ -1414,10 +1426,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C41" s="1">
         <v>2</v>
@@ -1434,7 +1446,7 @@
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1">
         <v>2</v>
@@ -1448,10 +1460,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C43" s="1">
         <v>2</v>
@@ -1465,10 +1477,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C44" s="1">
         <v>2</v>
@@ -1482,10 +1494,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C45" s="1">
         <v>2</v>
@@ -1499,10 +1511,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C46" s="1">
         <v>2</v>
@@ -1516,10 +1528,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
@@ -1533,10 +1545,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C48" s="1">
         <v>3</v>
@@ -1550,10 +1562,10 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C49" s="1">
         <v>3</v>
@@ -1567,10 +1579,10 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C50" s="1">
         <v>3</v>
@@ -1584,10 +1596,10 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C51" s="1">
         <v>3</v>
@@ -1601,10 +1613,10 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C52" s="1">
         <v>3</v>
@@ -1621,7 +1633,7 @@
         <v>2</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C53" s="1">
         <v>3</v>
@@ -1635,10 +1647,10 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C54" s="1">
         <v>3</v>
@@ -1652,10 +1664,10 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C55" s="1">
         <v>3</v>
@@ -1669,10 +1681,10 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C56" s="1">
         <v>3</v>
@@ -1689,7 +1701,7 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C57" s="1">
         <v>3</v>
@@ -1703,10 +1715,10 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C58" s="1">
         <v>3</v>
@@ -1720,10 +1732,10 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C59" s="1">
         <v>3</v>
@@ -1737,10 +1749,10 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C60" s="1">
         <v>3</v>
@@ -1757,7 +1769,7 @@
         <v>6</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C61" s="1">
         <v>3</v>
@@ -1770,130 +1782,130 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D62" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E62" s="3">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B63" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D63" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E63" s="3">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B64" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C62" s="1">
-        <v>4</v>
-      </c>
-      <c r="D62" s="3">
+      <c r="C64" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D64" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E64" s="3">
         <v>45810</v>
       </c>
-      <c r="E62" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B63" s="2" t="s">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B65" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D65" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E65" s="3">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D66" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E66" s="3">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D67" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E67" s="3">
+        <v>45810</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C63" s="1">
-        <v>4</v>
-      </c>
-      <c r="D63" s="3">
+      <c r="B68" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68" s="3">
+        <v>45803</v>
+      </c>
+      <c r="E68" s="3">
         <v>45810</v>
-      </c>
-      <c r="E63" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C64" s="1">
-        <v>4</v>
-      </c>
-      <c r="D64" s="3">
-        <v>45810</v>
-      </c>
-      <c r="E64" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C65" s="1">
-        <v>4</v>
-      </c>
-      <c r="D65" s="3">
-        <v>45810</v>
-      </c>
-      <c r="E65" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C66" s="1">
-        <v>4</v>
-      </c>
-      <c r="D66" s="3">
-        <v>45810</v>
-      </c>
-      <c r="E66" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C67" s="1">
-        <v>4</v>
-      </c>
-      <c r="D67" s="3">
-        <v>45810</v>
-      </c>
-      <c r="E67" s="3">
-        <v>45818</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="C68" s="1">
-        <v>4</v>
-      </c>
-      <c r="D68" s="3">
-        <v>45810</v>
-      </c>
-      <c r="E68" s="3">
-        <v>45818</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C69" s="1">
         <v>4</v>
@@ -1907,10 +1919,10 @@
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C70" s="1">
         <v>4</v>
@@ -1924,10 +1936,10 @@
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C71" s="1">
         <v>4</v>
@@ -1941,10 +1953,10 @@
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="C72" s="1">
         <v>4</v>
@@ -1958,10 +1970,10 @@
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C73" s="1">
         <v>4</v>
@@ -1975,10 +1987,10 @@
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C74" s="1">
         <v>4</v>
@@ -1992,10 +2004,10 @@
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C75" s="1">
         <v>4</v>
@@ -2009,10 +2021,10 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C76" s="1">
         <v>4</v>
@@ -2026,10 +2038,10 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="C77" s="1">
         <v>4</v>
@@ -2038,6 +2050,125 @@
         <v>45810</v>
       </c>
       <c r="E77" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C78" s="1">
+        <v>4</v>
+      </c>
+      <c r="D78" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E78" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A79" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B79" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C79" s="1">
+        <v>4</v>
+      </c>
+      <c r="D79" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E79" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B80" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C80" s="1">
+        <v>4</v>
+      </c>
+      <c r="D80" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E80" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A81" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C81" s="1">
+        <v>4</v>
+      </c>
+      <c r="D81" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E81" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C82" s="1">
+        <v>4</v>
+      </c>
+      <c r="D82" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E82" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A83" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C83" s="1">
+        <v>4</v>
+      </c>
+      <c r="D83" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E83" s="3">
+        <v>45818</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B84" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C84" s="1">
+        <v>4</v>
+      </c>
+      <c r="D84" s="3">
+        <v>45810</v>
+      </c>
+      <c r="E84" s="3">
         <v>45818</v>
       </c>
     </row>
@@ -2051,6 +2182,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3a1d6b35-d74b-4e6e-9e33-1d286005928a">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0d6b7251-971b-421d-9ba0-6b2023d693f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100AB947A98EBEFFA45B551653668971F36" ma:contentTypeVersion="23" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4a71894c677265028c25fea40c469a7d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3a1d6b35-d74b-4e6e-9e33-1d286005928a" xmlns:ns3="0d6b7251-971b-421d-9ba0-6b2023d693f9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3237d064db606537c4e696f73d4d905c" ns2:_="" ns3:_="">
     <xsd:import namespace="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
@@ -2305,27 +2456,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D7A6F5-4190-4B54-ACD3-37B34D18A408}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="0d6b7251-971b-421d-9ba0-6b2023d693f9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3a1d6b35-d74b-4e6e-9e33-1d286005928a">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0d6b7251-971b-421d-9ba0-6b2023d693f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A1A307-8C34-4E84-BA59-2F0A23A06A42}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57B7F710-491D-49B9-894A-18729FC96536}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2342,29 +2498,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44A1A307-8C34-4E84-BA59-2F0A23A06A42}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{15D7A6F5-4190-4B54-ACD3-37B34D18A408}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="3a1d6b35-d74b-4e6e-9e33-1d286005928a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="0d6b7251-971b-421d-9ba0-6b2023d693f9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>